<commit_message>
Update project mars User Story 1.xlsx
</commit_message>
<xml_diff>
--- a/project mars User Story 1.xlsx
+++ b/project mars User Story 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/39e9008c0d8a92b5/Pooja/Industry Connect/MVP Studio/Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/39e9008c0d8a92b5/Documents/GitHub/PoojaMVP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="471" documentId="8_{3F584EBA-4FE3-440B-87C6-D390C19C841F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95B2D9F0-BA09-4120-9CAC-F81F9167A031}"/>
+  <xr:revisionPtr revIDLastSave="472" documentId="8_{3F584EBA-4FE3-440B-87C6-D390C19C841F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95EE6222-48D6-4454-9924-D9E6D9EDFF31}"/>
   <bookViews>
-    <workbookView xWindow="12825" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{470A0961-32FE-4BC1-A90F-AB9F42D38E19}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="8170" xr2:uid="{470A0961-32FE-4BC1-A90F-AB9F42D38E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -833,13 +833,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4B3E61-09F7-4944-9D56-8BA80A2A966D}">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
     <col min="2" max="2" width="24.90625" style="1" customWidth="1"/>
     <col min="3" max="3" width="30.54296875" style="1" customWidth="1"/>
     <col min="4" max="4" width="27.453125" style="1" customWidth="1"/>

</xml_diff>